<commit_message>
Searching and Sorting_Day 1
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0594A13-4E22-4A5E-88A5-50E232333451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10CF8C0-0B4D-4609-93FD-D64017AE6528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="529">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1615,6 +1615,9 @@
   </si>
   <si>
     <t>map</t>
+  </si>
+  <si>
+    <t>Loop</t>
   </si>
 </sst>
 </file>
@@ -2060,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3372,9 +3375,11 @@
       <c r="B101" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C101" s="2"/>
+      <c r="C101" s="2" t="s">
+        <v>528</v>
+      </c>
       <c r="D101" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 2
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10CF8C0-0B4D-4609-93FD-D64017AE6528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27C9AD2-974E-464A-A429-022BC5D97551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="529">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1617,7 +1617,7 @@
     <t>map</t>
   </si>
   <si>
-    <t>Loop</t>
+    <t>Loop &amp; Search</t>
   </si>
 </sst>
 </file>
@@ -2064,7 +2064,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3389,9 +3389,11 @@
       <c r="B102" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C102" s="2"/>
+      <c r="C102" s="2" t="s">
+        <v>528</v>
+      </c>
       <c r="D102" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 3
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27C9AD2-974E-464A-A429-022BC5D97551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC5006F-9F0C-43B9-B826-3F10EBF34819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="529">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2064,7 +2064,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3403,9 +3403,11 @@
       <c r="B103" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C103" s="2"/>
+      <c r="C103" s="2" t="s">
+        <v>528</v>
+      </c>
       <c r="D103" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 4
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC5006F-9F0C-43B9-B826-3F10EBF34819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1C97FC-F481-4498-A99C-A5C6A94952B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="530">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1618,6 +1618,9 @@
   </si>
   <si>
     <t>Loop &amp; Search</t>
+  </si>
+  <si>
+    <t>Loop</t>
   </si>
 </sst>
 </file>
@@ -2064,7 +2067,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3417,9 +3420,11 @@
       <c r="B104" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C104" s="2"/>
+      <c r="C104" s="2" t="s">
+        <v>529</v>
+      </c>
       <c r="D104" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 5
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1C97FC-F481-4498-A99C-A5C6A94952B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3241F6A1-2A0F-4371-90CD-DDE51692ABF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="531">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1621,6 +1621,9 @@
   </si>
   <si>
     <t>Loop</t>
+  </si>
+  <si>
+    <t>Compare</t>
   </si>
 </sst>
 </file>
@@ -2067,7 +2070,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3434,9 +3437,11 @@
       <c r="B105" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C105" s="2"/>
+      <c r="C105" s="2" t="s">
+        <v>530</v>
+      </c>
       <c r="D105" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 6
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3241F6A1-2A0F-4371-90CD-DDE51692ABF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A4FC45-3FA0-4938-BDFA-47C181D71C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="532">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1624,6 +1624,9 @@
   </si>
   <si>
     <t>Compare</t>
+  </si>
+  <si>
+    <t>Ternary Search</t>
   </si>
 </sst>
 </file>
@@ -2070,7 +2073,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3451,9 +3454,11 @@
       <c r="B106" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C106" s="2"/>
+      <c r="C106" s="2" t="s">
+        <v>531</v>
+      </c>
       <c r="D106" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 7
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A4FC45-3FA0-4938-BDFA-47C181D71C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877DFCB8-3300-48C8-8B48-71352A3DF2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1442" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="532">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2073,7 +2073,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3468,9 +3468,11 @@
       <c r="B107" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C107" s="2"/>
+      <c r="C107" s="2" t="s">
+        <v>528</v>
+      </c>
       <c r="D107" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 8
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877DFCB8-3300-48C8-8B48-71352A3DF2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B52FC0-1EAE-418C-B72A-AEFDF69F2211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="532">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2072,8 +2072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3494,9 +3494,11 @@
       <c r="B109" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C109" s="2"/>
+      <c r="C109" s="2" t="s">
+        <v>528</v>
+      </c>
       <c r="D109" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 9
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B52FC0-1EAE-418C-B72A-AEFDF69F2211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBD040E-42BE-421B-8E0A-5BD605DBB33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="533">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1627,6 +1627,9 @@
   </si>
   <si>
     <t>Ternary Search</t>
+  </si>
+  <si>
+    <t>Two Pointer</t>
   </si>
 </sst>
 </file>
@@ -2073,7 +2076,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3508,9 +3511,11 @@
       <c r="B110" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C110" s="2"/>
+      <c r="C110" s="2" t="s">
+        <v>532</v>
+      </c>
       <c r="D110" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 10
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBD040E-42BE-421B-8E0A-5BD605DBB33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543222A3-E39D-4174-99FE-0C1A164F686B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="534">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1630,6 +1630,9 @@
   </si>
   <si>
     <t>Two Pointer</t>
+  </si>
+  <si>
+    <t>loops</t>
   </si>
 </sst>
 </file>
@@ -2076,7 +2079,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3525,9 +3528,11 @@
       <c r="B111" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C111" s="2"/>
+      <c r="C111" s="2" t="s">
+        <v>533</v>
+      </c>
       <c r="D111" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 11
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543222A3-E39D-4174-99FE-0C1A164F686B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A40C5DD-1EAC-42BE-BCAF-B62D50DD2BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="535">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1633,6 +1633,9 @@
   </si>
   <si>
     <t>loops</t>
+  </si>
+  <si>
+    <t>include exclude</t>
   </si>
 </sst>
 </file>
@@ -2078,8 +2081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3542,9 +3545,11 @@
       <c r="B112" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C112" s="2"/>
+      <c r="C112" s="2" t="s">
+        <v>534</v>
+      </c>
       <c r="D112" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 12
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A40C5DD-1EAC-42BE-BCAF-B62D50DD2BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B31F0A2-3402-448A-83B4-C8F4CF3A1FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="536">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1636,6 +1636,9 @@
   </si>
   <si>
     <t>include exclude</t>
+  </si>
+  <si>
+    <t>Three pointers</t>
   </si>
 </sst>
 </file>
@@ -2082,7 +2085,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3559,9 +3562,11 @@
       <c r="B113" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C113" s="2"/>
+      <c r="C113" s="2" t="s">
+        <v>535</v>
+      </c>
       <c r="D113" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 13
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B31F0A2-3402-448A-83B4-C8F4CF3A1FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D81436-934C-4855-866A-8297A3DBF6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="537">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1639,6 +1639,9 @@
   </si>
   <si>
     <t>Three pointers</t>
+  </si>
+  <si>
+    <t>Merge</t>
   </si>
 </sst>
 </file>
@@ -2085,7 +2088,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3576,9 +3579,11 @@
       <c r="B114" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C114" s="2"/>
+      <c r="C114" s="2" t="s">
+        <v>536</v>
+      </c>
       <c r="D114" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>

<commit_message>
Searching and Sorting_Day 14
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDY\JAVA\Final-450\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D81436-934C-4855-866A-8297A3DBF6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6AA283-9BA0-4637-9FB6-3DAAF23DDE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="537">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -2088,7 +2088,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="31.5" customHeight="1"/>
@@ -3593,9 +3593,11 @@
       <c r="B115" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C115" s="2"/>
+      <c r="C115" s="2" t="s">
+        <v>485</v>
+      </c>
       <c r="D115" s="8" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="31.5" customHeight="1">

</xml_diff>